<commit_message>
Add assertion to upload download test
</commit_message>
<xml_diff>
--- a/cypress/downloads/download.xlsx
+++ b/cypress/downloads/download.xlsx
@@ -37,7 +37,7 @@
     <t>Summer</t>
   </si>
   <si>
-    <t>Iphone</t>
+    <t>Apple</t>
   </si>
   <si>
     <t>Red</t>
@@ -543,7 +543,7 @@
         <v>17</v>
       </c>
       <c r="D6">
-        <v>399</v>
+        <v>150</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>

</xml_diff>